<commit_message>
mise à jour veilles et du projet_intranet
</commit_message>
<xml_diff>
--- a/t_competences/Tableau de synthèse - BTS SIO 2024_PORTOLLEAU.xlsx
+++ b/t_competences/Tableau de synthèse - BTS SIO 2024_PORTOLLEAU.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cbc9f0bb248b3f74/Bureau/Cours BTS/siteanais/Portfolio/t_competences/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cbc9f0bb248b3f74/Bureau/siteanais/Portfolio/t_competences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{04068206-C5EA-4954-A34F-87024FEAF2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="14_{04068206-C5EA-4954-A34F-87024FEAF2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C61E29C9-9ADB-48D6-B164-21A7E380B194}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -216,6 +216,12 @@
   <si>
     <t xml:space="preserve">▸Recenser et identifier les ressources numériques                                                           ▸ Gérer des sauvegardes                                 </t>
   </si>
+  <si>
+    <t>Projet Web - Intranet</t>
+  </si>
+  <si>
+    <t>06/01/2025 au 18/04/2025</t>
+  </si>
 </sst>
 </file>
 
@@ -627,7 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -722,6 +728,27 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -731,26 +758,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1145,7 +1154,7 @@
   <dimension ref="A1:AQ25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1164,56 +1173,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="32"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="34" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="2" t="s">
         <v>35</v>
       </c>
@@ -1225,22 +1234,22 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1263,8 +1272,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" s="8" customFormat="1" ht="324.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="39"/>
-      <c r="B7" s="40"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
@@ -1285,14 +1294,14 @@
       </c>
     </row>
     <row r="8" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
@@ -1306,9 +1315,7 @@
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="24" t="s">
-        <v>40</v>
-      </c>
+      <c r="F9" s="24"/>
       <c r="G9" s="21"/>
       <c r="H9" s="23"/>
     </row>
@@ -1353,12 +1360,18 @@
       <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:13" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="26"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
+      <c r="F12" s="21" t="s">
+        <v>40</v>
+      </c>
       <c r="G12" s="21"/>
       <c r="H12" s="22"/>
     </row>
@@ -1383,16 +1396,16 @@
       <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:13" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:13" s="8" customFormat="1" ht="109.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
@@ -1424,16 +1437,16 @@
       </c>
     </row>
     <row r="17" spans="1:8" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
     </row>
     <row r="18" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
@@ -1517,6 +1530,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A4:E4"/>
@@ -1524,11 +1542,6 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mise à jour veille + tableau compétences
</commit_message>
<xml_diff>
--- a/t_competences/Tableau de synthèse - BTS SIO 2024_PORTOLLEAU.xlsx
+++ b/t_competences/Tableau de synthèse - BTS SIO 2024_PORTOLLEAU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anais\OneDrive\Bureau\siteanais\Portfolio\t_competences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6131C1-C489-417F-B3F5-E7017224AB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC52F2E-F309-4C40-BAD7-B6CADAEA8465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$25</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -222,6 +222,12 @@
   <si>
     <t>▸Vérifier les conditions de la continuité d’un service informatique                                      ▸Exploiter des référentiels, normes et standards adoptés par le prestataire informatique</t>
   </si>
+  <si>
+    <t>PORTEFOLIO HTML/CSS/JS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Mettre en œuvre des outils et stratégies de veille informationnelle                                            - Gérer son identité professionnelle</t>
+  </si>
 </sst>
 </file>
 
@@ -633,7 +639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -727,9 +733,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1153,76 +1156,76 @@
   </sheetPr>
   <dimension ref="A1:AQ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="46" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="45.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="48.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="39.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="43" width="11.42578125" customWidth="1"/>
-    <col min="44" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="75.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="48.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="39.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="43" width="11.44140625" customWidth="1"/>
+    <col min="44" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="33"/>
-    </row>
-    <row r="2" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-    </row>
-    <row r="3" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+    <row r="4" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
       <c r="F4" s="2" t="s">
         <v>35</v>
       </c>
@@ -1233,23 +1236,23 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-    </row>
-    <row r="6" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+    </row>
+    <row r="6" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="40" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1271,9 +1274,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="8" customFormat="1" ht="324.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
-      <c r="B7" s="41"/>
+    <row r="7" spans="1:13" s="8" customFormat="1" ht="324.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
@@ -1293,17 +1296,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-    </row>
-    <row r="9" spans="1:13" s="8" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+    </row>
+    <row r="9" spans="1:13" s="8" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>30</v>
       </c>
@@ -1319,7 +1322,7 @@
       <c r="G9" s="21"/>
       <c r="H9" s="23"/>
     </row>
-    <row r="10" spans="1:13" s="8" customFormat="1" ht="97.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="8" customFormat="1" ht="97.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>39</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="8" customFormat="1" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="8" customFormat="1" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>26</v>
       </c>
@@ -1359,11 +1362,11 @@
       <c r="G11" s="21"/>
       <c r="H11" s="23"/>
     </row>
-    <row r="12" spans="1:13" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="25" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="21"/>
@@ -1375,17 +1378,21 @@
       <c r="G12" s="21"/>
       <c r="H12" s="22"/>
     </row>
-    <row r="13" spans="1:13" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
+    <row r="13" spans="1:13" s="8" customFormat="1" ht="73.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>51</v>
+      </c>
       <c r="B13" s="19"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
-      <c r="H13" s="22"/>
-    </row>
-    <row r="14" spans="1:13" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H13" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="19"/>
       <c r="C14" s="21"/>
@@ -1395,19 +1402,19 @@
       <c r="G14" s="21"/>
       <c r="H14" s="22"/>
     </row>
-    <row r="15" spans="1:13" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="36" t="s">
+    <row r="15" spans="1:13" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-    </row>
-    <row r="16" spans="1:13" s="8" customFormat="1" ht="109.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+    </row>
+    <row r="16" spans="1:13" s="8" customFormat="1" ht="109.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>28</v>
       </c>
@@ -1436,19 +1443,19 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="s">
+    <row r="17" spans="1:8" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-    </row>
-    <row r="18" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+    </row>
+    <row r="18" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
@@ -1458,7 +1465,7 @@
       <c r="G18" s="11"/>
       <c r="H18" s="16"/>
     </row>
-    <row r="19" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
@@ -1468,7 +1475,7 @@
       <c r="G19" s="11"/>
       <c r="H19" s="16"/>
     </row>
-    <row r="20" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
@@ -1478,7 +1485,7 @@
       <c r="G20" s="11"/>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="10"/>
       <c r="C21" s="11"/>
@@ -1488,7 +1495,7 @@
       <c r="G21" s="11"/>
       <c r="H21" s="16"/>
     </row>
-    <row r="22" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
@@ -1498,7 +1505,7 @@
       <c r="G22" s="11"/>
       <c r="H22" s="16"/>
     </row>
-    <row r="23" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
@@ -1508,7 +1515,7 @@
       <c r="G23" s="11"/>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="20"/>
       <c r="C24" s="17"/>
@@ -1518,7 +1525,7 @@
       <c r="G24" s="17"/>
       <c r="H24" s="18"/>
     </row>
-    <row r="25" spans="1:8" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>

</xml_diff>

<commit_message>
mise à jour compétences projet 1 - seconde année
</commit_message>
<xml_diff>
--- a/t_competences/Tableau de synthèse - BTS SIO 2024_PORTOLLEAU.xlsx
+++ b/t_competences/Tableau de synthèse - BTS SIO 2024_PORTOLLEAU.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anais\OneDrive\Bureau\siteanais\Portfolio\t_competences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3E1FDF-9566-4779-A2AE-A40D8B0B4BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F5D6F9-23CC-47E4-8D01-A636CE6B878C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -223,6 +223,15 @@
     <t xml:space="preserve">
 ▸Traiter des demandes concernant les applications                                                                </t>
   </si>
+  <si>
+    <t>15/09/2025 au 13/10/2025</t>
+  </si>
+  <si>
+    <t>Projet Web 2 - Site Resto</t>
+  </si>
+  <si>
+    <t>▸Accompagner les utilisateurs dans la mise en place d’un service  ▸Déployer un service</t>
+  </si>
 </sst>
 </file>
 
@@ -231,7 +240,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* \-??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -334,8 +343,15 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -630,11 +646,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -690,9 +707,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -730,6 +744,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -739,30 +771,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1152,8 +1173,8 @@
   </sheetPr>
   <dimension ref="A1:AQ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:H17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1172,83 +1193,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="33"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
       <c r="F4" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="29" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="36" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1271,8 +1292,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" s="8" customFormat="1" ht="324.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="41"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
@@ -1293,161 +1314,169 @@
       </c>
     </row>
     <row r="8" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="97.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="23" t="s">
+      <c r="F10" s="23"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="22" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="8" customFormat="1" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="22"/>
     </row>
     <row r="12" spans="1:13" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21" t="s">
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:13" s="8" customFormat="1" ht="73.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="23" t="s">
+      <c r="B13" s="41"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="22"/>
-    </row>
-    <row r="15" spans="1:13" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+    <row r="14" spans="1:13" s="8" customFormat="1" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="20"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="21"/>
+    </row>
+    <row r="15" spans="1:13" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
     </row>
     <row r="16" spans="1:13" s="8" customFormat="1" ht="109.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="23" t="s">
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="29" t="s">
+      <c r="I16" s="28" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1511,7 +1540,7 @@
     </row>
     <row r="24" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
-      <c r="B24" s="20"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
@@ -1531,6 +1560,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A4:E4"/>
@@ -1538,11 +1572,6 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mise à jour compétences
</commit_message>
<xml_diff>
--- a/t_competences/Tableau de synthèse - BTS SIO 2024_PORTOLLEAU.xlsx
+++ b/t_competences/Tableau de synthèse - BTS SIO 2024_PORTOLLEAU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anais\OneDrive\Bureau\siteanais\Portfolio\t_competences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F5D6F9-23CC-47E4-8D01-A636CE6B878C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{34F75D9C-4FAB-4279-B9B4-691CBE1EE43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -217,13 +217,6 @@
     <t xml:space="preserve">▸Recenser et identifier les ressources numériques                                        ▸Mettre en place et vérifier les niveaux d’habilitation associés à un service                                                                              </t>
   </si>
   <si>
-    <t xml:space="preserve">▸Gérer des sauvegardes                                                                                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-▸Traiter des demandes concernant les applications                                                                </t>
-  </si>
-  <si>
     <t>15/09/2025 au 13/10/2025</t>
   </si>
   <si>
@@ -364,7 +357,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -642,6 +635,21 @@
       </top>
       <bottom style="medium">
         <color rgb="FF4A452A"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF4A452A"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF4A452A"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF4A452A"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -651,7 +659,7 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -744,6 +752,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -762,23 +788,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1173,8 +1184,8 @@
   </sheetPr>
   <dimension ref="A1:AQ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1193,56 +1204,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="38"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
       <c r="F4" s="2" t="s">
         <v>34</v>
       </c>
@@ -1254,22 +1265,22 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="42" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1292,8 +1303,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" s="8" customFormat="1" ht="324.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
@@ -1314,14 +1325,14 @@
       </c>
     </row>
     <row r="8" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
@@ -1401,7 +1412,7 @@
       <c r="A13" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="41"/>
+      <c r="B13" s="44"/>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
@@ -1413,33 +1424,33 @@
     </row>
     <row r="14" spans="1:13" s="8" customFormat="1" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>50</v>
       </c>
       <c r="C14" s="20"/>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="33" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="23"/>
       <c r="G14" s="23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:13" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
     </row>
     <row r="16" spans="1:13" s="8" customFormat="1" ht="109.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
@@ -1448,12 +1459,8 @@
       <c r="B16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>51</v>
-      </c>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="23" t="s">
         <v>32</v>
       </c>
@@ -1467,16 +1474,16 @@
       </c>
     </row>
     <row r="17" spans="1:8" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
     </row>
     <row r="18" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1560,11 +1567,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A4:E4"/>
@@ -1572,6 +1574,11 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
veille phisihing enlevé + mise à jour des 3 veilles
</commit_message>
<xml_diff>
--- a/t_competences/Tableau de synthèse - BTS SIO 2024_PORTOLLEAU.xlsx
+++ b/t_competences/Tableau de synthèse - BTS SIO 2024_PORTOLLEAU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anais\OneDrive\Bureau\siteanais\Portfolio\t_competences\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cbc9f0bb248b3f74/Bureau/siteanais/Portfolio/t_competences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34F75D9C-4FAB-4279-B9B4-691CBE1EE43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{34F75D9C-4FAB-4279-B9B4-691CBE1EE43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72FE344D-CB9D-40FB-B566-C79F8A2C99B0}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -187,12 +187,6 @@
     <t>Adresse URL du portfolio :  https://anaisprt44.github.io/Portfolio/</t>
   </si>
   <si>
-    <t xml:space="preserve">▸Développer son projet professionnel </t>
-  </si>
-  <si>
-    <t>▸Mettre en place son environnement d’apprentissage personnel                                     ▸Mettre en oeuvre des outils et stratégies de veille informationnelle                                                                                                              ▸Gérer son identité professionnelle</t>
-  </si>
-  <si>
     <t>Projet Web - Intranet</t>
   </si>
   <si>
@@ -205,9 +199,6 @@
     <t>PORTEFOLIO HTML/CSS/JS</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Mettre en œuvre des outils et stratégies de veille informationnelle                                            - Gérer son identité professionnelle</t>
-  </si>
-  <si>
     <t xml:space="preserve">                                                                                              ▸Vérifier le respect des règles d’utilisation des ressources numériques</t>
   </si>
   <si>
@@ -224,6 +215,12 @@
   </si>
   <si>
     <t>▸Accompagner les utilisateurs dans la mise en place d’un service  ▸Déployer un service</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Mettre en œuvre des outils et stratégies de veille informationnelle                                            </t>
+  </si>
+  <si>
+    <t>▸Mettre en place son environnement d’apprentissage personnel                                                                                                                                                ▸Gérer son identité professionnelle</t>
   </si>
 </sst>
 </file>
@@ -758,6 +755,30 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -766,30 +787,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1184,8 +1181,8 @@
   </sheetPr>
   <dimension ref="A1:AQ25"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1204,56 +1201,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="34"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="36" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
       <c r="F4" s="2" t="s">
         <v>34</v>
       </c>
@@ -1265,22 +1262,22 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
     </row>
     <row r="6" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="40" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1303,8 +1300,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" s="8" customFormat="1" ht="324.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
@@ -1325,14 +1322,14 @@
       </c>
     </row>
     <row r="8" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
@@ -1342,7 +1339,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -1358,7 +1355,7 @@
         <v>24</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>29</v>
@@ -1368,9 +1365,7 @@
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="20"/>
-      <c r="H10" s="22" t="s">
-        <v>40</v>
-      </c>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:13" s="8" customFormat="1" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
@@ -1380,7 +1375,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>31</v>
@@ -1392,13 +1387,13 @@
     </row>
     <row r="12" spans="1:13" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
@@ -1410,24 +1405,24 @@
     </row>
     <row r="13" spans="1:13" s="8" customFormat="1" ht="73.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="44"/>
+        <v>43</v>
+      </c>
+      <c r="B13" s="34"/>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
       <c r="H13" s="22" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="8" customFormat="1" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="33" t="s">
@@ -1436,21 +1431,21 @@
       <c r="E14" s="20"/>
       <c r="F14" s="23"/>
       <c r="G14" s="23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:13" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
     </row>
     <row r="16" spans="1:13" s="8" customFormat="1" ht="109.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
@@ -1467,23 +1462,23 @@
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
       <c r="H16" s="22" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="I16" s="28" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
     </row>
     <row r="18" spans="1:8" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1567,6 +1562,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A4:E4"/>
@@ -1574,11 +1574,6 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>